<commit_message>
new daily model restuls
</commit_message>
<xml_diff>
--- a/data/results/daily_model/daily_model_results.xlsx
+++ b/data/results/daily_model/daily_model_results.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,11 +444,51 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
+          <t>TOTALENERGIES SE</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>64.36430317848411</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>FMC CORP</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>75.67237163814181</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>BP PLC</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>93.7041564792176</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>STORA ENSO</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>91.99266503667481</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
           <t>BHP GROUP</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>94.0234134319162</v>
+      <c r="B6" t="n">
+        <v>93.27628361858191</v>
       </c>
     </row>
   </sheetData>
@@ -462,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,15 +513,10 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Cross-Correlation</t>
+          <t>Pearson Correlation</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Pearson Correlation (need to stationarize)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>P-value</t>
         </is>
@@ -490,26 +525,66 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
+          <t>TOTALENERGIES SE</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01566256551086196</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.600871449251472</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>FMC CORP</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.01770014237732665</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5110361495306047</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>BP PLC</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.009638066301792383</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.7001561347054477</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>STORA ENSO</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.01530076064468157</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5439945818950872</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
           <t>BHP GROUP</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>(array([ 2.35795909e-02, -3.80925242e-03,  4.43276351e-02, ...,
-       -5.87639818e-05, -2.92548581e-05,  1.44473427e-05]), array([[-0.02572865,  0.07288784],
-       [-0.0531175 ,  0.04549899],
-       [-0.00498061,  0.09363588],
-       ...,
-       [-0.04936701,  0.04924948],
-       [-0.0493375 ,  0.04927899],
-       [-0.0492938 ,  0.04932269]]))</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0.02357959089236476</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.3489341767463884</v>
+      <c r="B6" t="n">
+        <v>-0.01422839565825462</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5719727335739155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>